<commit_message>
- Behaviour_box_small:         - Added holes to corners of base for mounting to floor
- Behaviour_box_small/nine_poke_panel
        - Moved pokes 5mm upwards.
        - Changed design of poke assemly plastic parts to improve optical isolation of LEDs from different pokes.

- Nine_poke/solenoid_driver_1_0
        - Added picoblade cable to BOM

- Sound attenuating chamber small:
        -  Changed resistor for LED driver.
        -  Changed model of ball head mount
</commit_message>
<xml_diff>
--- a/Behaviour_box_small/back_panel_variants/nine_poke_panel/nine_poke_panel_BOM.xlsx
+++ b/Behaviour_box_small/back_panel_variants/nine_poke_panel/nine_poke_panel_BOM.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48668D0A-BB27-4567-A1A8-A9E1DD762AF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Part</t>
   </si>
@@ -34,15 +35,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>back_opal_030_5mm_acrylic</t>
-  </si>
-  <si>
     <t>cover_black_1.5mm_HIPS</t>
   </si>
   <si>
-    <t>back_inserts_black_1.5mm_HIPS</t>
-  </si>
-  <si>
     <t>Mounting hardware</t>
   </si>
   <si>
@@ -161,12 +156,21 @@
   </si>
   <si>
     <t>5mm opal 030 acrylic</t>
+  </si>
+  <si>
+    <t>ports_white_5mm</t>
+  </si>
+  <si>
+    <t>ports_opal030_5mm</t>
+  </si>
+  <si>
+    <t>ports_black_1.5mm_HIPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,10 +214,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -308,6 +313,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -343,6 +365,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -518,11 +557,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -559,305 +598,318 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="C5" s="3">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
+      <c r="F12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>1419607</v>
+      <c r="A13" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>2506007</v>
+        <v>1419607</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>1733403</v>
+        <v>2506007</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G16">
-        <v>359154</v>
+        <v>1733403</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>1420717</v>
+        <v>359154</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>1420717</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>1420788</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>1420788</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="G20" s="2">
+        <v>2474926</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C21">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="2">
-        <v>2474926</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20">
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22">
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23">
         <v>1867858</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D3:E3"/>
+  <mergeCells count="5">
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- Updated the design files for the 9 port panel to use plastic parts with better isolation of stimulus LED light between ports.
</commit_message>
<xml_diff>
--- a/Behaviour_box_small/back_panel_variants/nine_poke_panel/nine_poke_panel_BOM.xlsx
+++ b/Behaviour_box_small/back_panel_variants/nine_poke_panel/nine_poke_panel_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48668D0A-BB27-4567-A1A8-A9E1DD762AF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DC3A55-4B04-4E5B-8D60-0859C679C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="1665" windowWidth="13635" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Part</t>
   </si>
@@ -72,15 +72,6 @@
   </si>
   <si>
     <t>M3 round spacer 5x2mm</t>
-  </si>
-  <si>
-    <t>M3 hex spacer 3mm</t>
-  </si>
-  <si>
-    <t>HARWIN</t>
-  </si>
-  <si>
-    <t>R30-9400300</t>
   </si>
   <si>
     <t>PCBs</t>
@@ -558,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -599,31 +590,31 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3">
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -635,19 +626,19 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" s="4"/>
     </row>
@@ -673,24 +664,24 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
@@ -698,19 +689,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -720,7 +711,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -780,126 +771,106 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
       <c r="G17">
-        <v>359154</v>
+        <v>1420717</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
       </c>
       <c r="G18">
-        <v>1420717</v>
+        <v>1420788</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C19">
+      <c r="F19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="G19" s="2">
+        <v>2474926</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="F19" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G19">
-        <v>1420788</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="2">
-        <v>2474926</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23">
+      <c r="G22">
         <v>1867858</v>
       </c>
     </row>

</xml_diff>